<commit_message>
befor merg with itzik
</commit_message>
<xml_diff>
--- a/data/apprentice_enter_lab.xlsx
+++ b/data/apprentice_enter_lab.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\OZKL\T_H\backflask---T.H-app\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F91D68D-7F9B-4908-BDEE-5897D4042BA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87BC8365-0C7D-4F68-A476-C87D16C6BE23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-80" yWindow="-80" windowWidth="19360" windowHeight="10360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="113">
   <si>
     <t>שם</t>
   </si>
@@ -230,9 +230,6 @@
   </si>
   <si>
     <t>בני דוד עלי</t>
-  </si>
-  <si>
-    <t>בני דוד הבקעה</t>
   </si>
   <si>
     <t xml:space="preserve">בני דוד דרך אבות </t>
@@ -371,7 +368,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -383,13 +380,6 @@
       <u/>
       <sz val="10"/>
       <color theme="1"/>
-      <name val="David"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
       <name val="David"/>
       <family val="2"/>
     </font>
@@ -471,30 +461,27 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="2"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -840,8 +827,8 @@
   <sheetPr codeName="Sheet 1"/>
   <dimension ref="A1:AI4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="O4" sqref="O4"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="T3" sqref="T3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -925,43 +912,43 @@
       <c r="X1" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="6" t="s">
+      <c r="Y1" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="Z1" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="Z1" s="6" t="s">
+      <c r="AA1" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="AA1" s="6" t="s">
+      <c r="AB1" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="AB1" s="6" t="s">
+      <c r="AC1" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="AC1" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="AD1" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="AE1" s="6" t="s">
+      <c r="AD1" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="AE1" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="AF1" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="AF1" s="6" t="s">
+      <c r="AG1" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="AG1" s="8" t="s">
+      <c r="AH1" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="AH1" s="6" t="s">
+      <c r="AI1" s="5" t="s">
         <v>106</v>
-      </c>
-      <c r="AI1" s="6" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="2" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B2">
         <v>549247615</v>
@@ -969,8 +956,8 @@
       <c r="C2" t="s">
         <v>24</v>
       </c>
-      <c r="D2" s="4">
-        <v>544816491</v>
+      <c r="D2" s="3">
+        <v>523301800</v>
       </c>
       <c r="E2" t="s">
         <v>57</v>
@@ -997,13 +984,13 @@
         <v>31</v>
       </c>
       <c r="M2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="N2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="O2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="P2" t="s">
         <v>34</v>
@@ -1030,25 +1017,25 @@
         <v>25</v>
       </c>
       <c r="X2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="Y2" t="s">
-        <v>76</v>
-      </c>
-      <c r="Z2" s="7" t="s">
-        <v>100</v>
+        <v>75</v>
+      </c>
+      <c r="Z2" s="6" t="s">
+        <v>99</v>
       </c>
       <c r="AA2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="AB2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="AC2" t="s">
         <v>30</v>
       </c>
-      <c r="AD2" s="7" t="s">
-        <v>100</v>
+      <c r="AD2" s="6" t="s">
+        <v>99</v>
       </c>
       <c r="AE2" t="s">
         <v>40</v>
@@ -1068,7 +1055,7 @@
     </row>
     <row r="3" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B3">
         <v>549247614</v>
@@ -1076,17 +1063,17 @@
       <c r="C3" t="s">
         <v>41</v>
       </c>
-      <c r="D3" s="5">
-        <v>544816492</v>
+      <c r="D3" s="3">
+        <v>523301803</v>
       </c>
       <c r="E3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F3" t="s">
         <v>43</v>
       </c>
-      <c r="G3" s="2" t="s">
-        <v>69</v>
+      <c r="G3" s="1" t="s">
+        <v>68</v>
       </c>
       <c r="H3" t="s">
         <v>44</v>
@@ -1110,7 +1097,7 @@
         <v>33</v>
       </c>
       <c r="O3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="P3" t="s">
         <v>50</v>
@@ -1119,10 +1106,10 @@
         <v>51</v>
       </c>
       <c r="R3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="S3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="T3" t="s">
         <v>52</v>
@@ -1137,25 +1124,25 @@
         <v>42</v>
       </c>
       <c r="X3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="Y3" t="s">
-        <v>77</v>
-      </c>
-      <c r="Z3" s="7" t="s">
-        <v>79</v>
+        <v>76</v>
+      </c>
+      <c r="Z3" s="6" t="s">
+        <v>78</v>
       </c>
       <c r="AA3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="AB3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="AC3" t="s">
         <v>47</v>
       </c>
-      <c r="AD3" s="7" t="s">
-        <v>101</v>
+      <c r="AD3" s="6" t="s">
+        <v>100</v>
       </c>
       <c r="AE3" t="s">
         <v>54</v>
@@ -1175,7 +1162,7 @@
     </row>
     <row r="4" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B4">
         <v>549247613</v>
@@ -1183,17 +1170,17 @@
       <c r="C4" t="s">
         <v>55</v>
       </c>
-      <c r="D4" s="5">
-        <v>544816493</v>
+      <c r="D4" s="4">
+        <v>523301801</v>
       </c>
       <c r="E4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F4" t="s">
-        <v>95</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>70</v>
+        <v>94</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>69</v>
       </c>
       <c r="H4" t="s">
         <v>58</v>
@@ -1211,13 +1198,13 @@
         <v>62</v>
       </c>
       <c r="M4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="N4" t="s">
         <v>63</v>
       </c>
       <c r="O4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="P4" t="s">
         <v>64</v>
@@ -1226,7 +1213,7 @@
         <v>32</v>
       </c>
       <c r="R4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="S4" t="s">
         <v>37</v>
@@ -1244,25 +1231,25 @@
         <v>56</v>
       </c>
       <c r="X4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="Y4" t="s">
-        <v>78</v>
-      </c>
-      <c r="Z4" s="7" t="s">
-        <v>80</v>
+        <v>77</v>
+      </c>
+      <c r="Z4" s="6" t="s">
+        <v>79</v>
       </c>
       <c r="AA4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="AB4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="AC4" t="s">
         <v>61</v>
       </c>
-      <c r="AD4" s="7" t="s">
-        <v>102</v>
+      <c r="AD4" s="6" t="s">
+        <v>101</v>
       </c>
       <c r="AE4" t="s">
         <v>67</v>
@@ -1277,12 +1264,12 @@
         <v>3</v>
       </c>
       <c r="AI4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="B1:B4" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
-  <phoneticPr fontId="6" type="noConversion"/>
+  <phoneticPr fontId="5" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="Z2" r:id="rId1" xr:uid="{5B435670-86E0-45A8-90D3-D18D08026C23}"/>
     <hyperlink ref="Z3" r:id="rId2" xr:uid="{B865A5ED-7E60-4EC5-B675-4DF8CDCF1ADF}"/>

</xml_diff>

<commit_message>
befor ahrai tohnit noti
</commit_message>
<xml_diff>
--- a/data/apprentice_enter_lab.xlsx
+++ b/data/apprentice_enter_lab.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\OZKL\T_H\backflask---T.H-app\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37314BEF-46C6-4E90-8227-042D2C8BA4A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDDD68FE-EAF4-4D20-9436-F1267D63AF6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{EE0135EA-A3CD-4A7C-A703-7BC851E2A15A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="80">
   <si>
     <t>חניך 1</t>
   </si>
@@ -269,10 +269,13 @@
     <t>מרכז</t>
   </si>
   <si>
-    <t>תשרי</t>
-  </si>
-  <si>
     <t xml:space="preserve">בני דוד דרך אבות </t>
+  </si>
+  <si>
+    <t>יא תשרי</t>
+  </si>
+  <si>
+    <t>דרום</t>
   </si>
 </sst>
 </file>
@@ -373,7 +376,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -393,6 +396,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -711,8 +717,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88626C00-A879-449E-8101-7BD32B33290B}">
   <dimension ref="A1:AN3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AC1" workbookViewId="0">
-      <selection activeCell="AL2" sqref="AL2"/>
+    <sheetView tabSelected="1" topLeftCell="U1" workbookViewId="0">
+      <selection activeCell="AK2" sqref="AK2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -863,7 +869,7 @@
         <v>313387345</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>4</v>
@@ -950,10 +956,10 @@
         <v>73</v>
       </c>
       <c r="AK2" s="5" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="AL2" s="8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="AM2" s="7">
         <v>549247616</v>
@@ -1074,8 +1080,8 @@
       <c r="AL3" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="AM3" s="7">
-        <v>549247615</v>
+      <c r="AM3" s="9">
+        <v>549247617</v>
       </c>
       <c r="AN3" s="2" t="s">
         <v>75</v>

</xml_diff>

<commit_message>
gift and maddadim setting 2
</commit_message>
<xml_diff>
--- a/data/apprentice_enter_lab.xlsx
+++ b/data/apprentice_enter_lab.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\OZKL\T_H\backflask---T.H-app\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0345236-0C23-4741-A4DD-49EF5F81F160}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC28DB19-B76F-4528-A19F-4E803F064240}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -267,9 +267,6 @@
     <t>הייטק</t>
   </si>
   <si>
-    <t>חיל שריון</t>
-  </si>
-  <si>
     <t>צנחנים</t>
   </si>
   <si>
@@ -297,9 +294,6 @@
     <t>אוניברסיטת בן-גוריון בנגב</t>
   </si>
   <si>
-    <t>חי״ר</t>
-  </si>
-  <si>
     <t>גבעתי</t>
   </si>
   <si>
@@ -325,6 +319,12 @@
   </si>
   <si>
     <t>נשוי</t>
+  </si>
+  <si>
+    <t>סיירות</t>
+  </si>
+  <si>
+    <t>גדודים</t>
   </si>
 </sst>
 </file>
@@ -711,8 +711,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BA90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+    <sheetView tabSelected="1" topLeftCell="AN1" workbookViewId="0">
+      <selection activeCell="AQ3" sqref="AQ3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15" customHeight="1"/>
@@ -945,10 +945,10 @@
         <v>117474</v>
       </c>
       <c r="J2" s="20" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="L2" s="2" t="s">
         <v>60</v>
@@ -1002,7 +1002,7 @@
         <v>117474</v>
       </c>
       <c r="AC2" s="9" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="AD2" s="9" t="s">
         <v>70</v>
@@ -1044,19 +1044,19 @@
         <v>79</v>
       </c>
       <c r="AQ2" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="AR2" s="2" t="s">
         <v>80</v>
-      </c>
-      <c r="AR2" s="2" t="s">
-        <v>81</v>
       </c>
       <c r="AS2" s="10">
         <v>888</v>
       </c>
       <c r="AT2" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="AU2" s="11" t="s">
         <v>82</v>
-      </c>
-      <c r="AU2" s="11" t="s">
-        <v>83</v>
       </c>
       <c r="AV2" s="8">
         <v>117474</v>
@@ -1065,10 +1065,10 @@
         <v>117474</v>
       </c>
       <c r="AX2" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="AY2" s="19" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="AZ2" s="12">
         <v>549247616</v>
@@ -1076,7 +1076,7 @@
     </row>
     <row r="3" spans="1:53" ht="24" customHeight="1">
       <c r="A3" s="5" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B3" s="10" t="s">
         <v>53</v>
@@ -1092,16 +1092,16 @@
         <v>56</v>
       </c>
       <c r="G3" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="H3" s="2" t="s">
         <v>85</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>86</v>
       </c>
       <c r="I3" s="8">
         <v>117474</v>
       </c>
       <c r="J3" s="20" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="K3" s="1" t="s">
         <v>59</v>
@@ -1110,7 +1110,7 @@
         <v>60</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="N3" s="2" t="s">
         <v>62</v>
@@ -1140,7 +1140,7 @@
         <v>69</v>
       </c>
       <c r="W3" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="X3" s="7" t="s">
         <v>68</v>
@@ -1149,10 +1149,10 @@
         <v>65</v>
       </c>
       <c r="Z3" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="AA3" s="2" t="s">
         <v>85</v>
-      </c>
-      <c r="AA3" s="2" t="s">
-        <v>86</v>
       </c>
       <c r="AB3" s="8">
         <v>117474</v>
@@ -1174,7 +1174,7 @@
         <v>72</v>
       </c>
       <c r="AI3" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="AJ3" s="2" t="s">
         <v>74</v>
@@ -1192,25 +1192,25 @@
         <v>77</v>
       </c>
       <c r="AO3" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="AP3" s="2" t="s">
         <v>79</v>
       </c>
       <c r="AQ3" s="2" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="AR3" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="AS3" s="10">
         <v>999</v>
       </c>
       <c r="AT3" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="AU3" s="11" t="s">
         <v>82</v>
-      </c>
-      <c r="AU3" s="11" t="s">
-        <v>83</v>
       </c>
       <c r="AV3" s="8">
         <v>117475</v>
@@ -1219,10 +1219,10 @@
         <v>117475</v>
       </c>
       <c r="AX3" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="AY3" s="19" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="AZ3" s="12">
         <v>549247616</v>
@@ -1285,7 +1285,7 @@
     </row>
     <row r="13" spans="1:53" ht="15.5">
       <c r="G13" s="18" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="AN13" s="17"/>
       <c r="AO13" s="14"/>
@@ -1326,7 +1326,7 @@
     </row>
     <row r="22" spans="7:53" ht="15.5">
       <c r="G22" s="18" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="AO22" s="16"/>
       <c r="BA22" s="13"/>
@@ -1550,9 +1550,6 @@
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="L2:L3" xr:uid="{00000000-0002-0000-0000-000004000000}">
       <formula1>"בשירות סדיר,קבע,משוחרר,בטיול אחרי צבא"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="AQ2:AQ3" xr:uid="{00000000-0002-0000-0000-000005000000}">
-      <formula1>"חי״ר,חיל שריון,חיל הים,חיל האוויר,סיירות,חיל תותחנים,חיל הנדסה,מודיעין"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="K2:K3" xr:uid="{00000000-0002-0000-0000-000006000000}">
       <formula1>"רווק,נשוי,גרוש"</formula1>
@@ -1572,6 +1569,9 @@
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="AY2:AY3" xr:uid="{6DC33454-2E06-4849-A10A-ABACE9D3C422}">
       <formula1>"אשכול דרום,אשכול מרכז,אשכול צפון,אשכול בני - דוד"</formula1>
     </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="AQ1:AQ1048576" xr:uid="{38CA151A-D39E-4370-8916-F9CFAA7E418E}">
+      <formula1>"סיירות,גדודים"</formula1>
+    </dataValidation>
   </dataValidations>
   <hyperlinks>
     <hyperlink ref="J2" r:id="rId1" xr:uid="{3AE54CEE-7EC2-40FF-8386-CE468EEED634}"/>

</xml_diff>